<commit_message>
version final para vercel
</commit_message>
<xml_diff>
--- a/data/terceros.xlsx
+++ b/data/terceros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camon\Documents\SYNC BI\NEVOX FARMA\Egresos\pdf-terceros-mailer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7E6E7B-0F6D-4B7F-8856-9C57A8C83C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1669109A-4080-483E-8B70-2CFD5F61F5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25440" yWindow="3360" windowWidth="21600" windowHeight="11235" xr2:uid="{CF22D517-537F-46EE-916E-5B570FD9473C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CF22D517-537F-46EE-916E-5B570FD9473C}"/>
   </bookViews>
   <sheets>
     <sheet name="Consulta General Xirux" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Consulta General Xirux'!$A$1:$C$7809</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Nit</t>
   </si>
@@ -46,15 +47,6 @@
   </si>
   <si>
     <t>CARVAJAL TECNOLOGIA Y SERVICIOS S A</t>
-  </si>
-  <si>
-    <t>carlos.montero@syncbi.net</t>
-  </si>
-  <si>
-    <t>desarrollo.fya@nevoxfarma.com</t>
-  </si>
-  <si>
-    <t>gestor.fya@nevoxfarma.com</t>
   </si>
 </sst>
 </file>
@@ -424,13 +416,13 @@
   <dimension ref="A1:C7809"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="76.77734375" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.21875" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -459,7 +451,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -470,7 +462,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -481,7 +473,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -39508,11 +39500,10 @@
   <autoFilter ref="A1:C7809" xr:uid="{7B82156A-906E-4D1D-B6BE-15E1A8DAA1D7}"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{39E1E8EE-F3A5-4C47-AD75-A4A45F7A37DE}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{7DE84A61-4BF3-497E-9414-24CBFCBEBE29}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{078D2991-BD33-4861-91E5-7145B010C66C}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{8DB12554-491B-4BEB-8693-6A2003481CE1}"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="camonteroperez@gmail.com" xr:uid="{7ACDA7A5-92FA-481A-B7ED-4EEE1906E432}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Informacion publica</oddFooter>
   </headerFooter>

</xml_diff>